<commit_message>
Clean repo pass 1
</commit_message>
<xml_diff>
--- a/DataFormat/RawData/UDZ_ungulates_2018_2019.xlsx
+++ b/DataFormat/RawData/UDZ_ungulates_2018_2019.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim O'Brien\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farrmt\Documents\HMSNO\DataFormat\EditedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D18AC5A-6125-4E8B-A6FA-2D7C1EF96798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="deployments" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'C. harveyi'!$A$1:$J$121</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">C.spadix!$A$1:$J$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'C.spadix'!$A$1:$J$121</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">N.moschatus!$A$1:$J$121</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2212" uniqueCount="81">
   <si>
     <t>Sampling.Unit.Name</t>
   </si>
@@ -282,7 +283,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,7 +598,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2623,10 +2624,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A177" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -6955,7 +6956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11569,16 +11570,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J121"/>
+  <autoFilter ref="A1:J121" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1:M122"/>
     </sheetView>
   </sheetViews>
@@ -16191,16 +16192,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J121"/>
+  <autoFilter ref="A1:J121" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A112" workbookViewId="0">
       <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
@@ -20811,17 +20812,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J121"/>
+  <autoFilter ref="A1:J121" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20879,6 +20880,9 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
       <c r="D2">
         <v>0</v>
       </c>
@@ -20914,6 +20918,9 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
       <c r="D3">
         <v>0</v>
       </c>
@@ -20949,6 +20956,9 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
       <c r="D4">
         <v>0</v>
       </c>
@@ -20984,6 +20994,9 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
       <c r="D5">
         <v>0</v>
       </c>
@@ -21019,6 +21032,9 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
       <c r="D6">
         <v>0</v>
       </c>
@@ -21054,6 +21070,9 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
       <c r="D7">
         <v>0</v>
       </c>
@@ -21089,6 +21108,9 @@
       <c r="B8" t="s">
         <v>10</v>
       </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
       <c r="D8">
         <v>0</v>
       </c>
@@ -21124,6 +21146,9 @@
       <c r="B9" t="s">
         <v>11</v>
       </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
       <c r="D9">
         <v>0</v>
       </c>
@@ -21159,6 +21184,9 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
       <c r="D10">
         <v>0</v>
       </c>
@@ -21194,6 +21222,9 @@
       <c r="B11" t="s">
         <v>13</v>
       </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
       <c r="D11">
         <v>0</v>
       </c>
@@ -21229,6 +21260,9 @@
       <c r="B12" t="s">
         <v>14</v>
       </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
       <c r="D12">
         <v>0</v>
       </c>
@@ -21264,6 +21298,9 @@
       <c r="B13" t="s">
         <v>15</v>
       </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
       <c r="D13">
         <v>0</v>
       </c>
@@ -21299,6 +21336,9 @@
       <c r="B14" t="s">
         <v>16</v>
       </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
       <c r="D14">
         <v>0</v>
       </c>
@@ -21410,6 +21450,9 @@
       <c r="B17" t="s">
         <v>19</v>
       </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
       <c r="D17">
         <v>0</v>
       </c>
@@ -21445,6 +21488,9 @@
       <c r="B18" t="s">
         <v>20</v>
       </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
       <c r="D18">
         <v>0</v>
       </c>
@@ -21480,6 +21526,9 @@
       <c r="B19" t="s">
         <v>62</v>
       </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
       <c r="D19" t="s">
         <v>80</v>
       </c>
@@ -21515,6 +21564,9 @@
       <c r="B20" t="s">
         <v>21</v>
       </c>
+      <c r="C20" t="s">
+        <v>71</v>
+      </c>
       <c r="D20">
         <v>0</v>
       </c>
@@ -21550,6 +21602,9 @@
       <c r="B21" t="s">
         <v>22</v>
       </c>
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
       <c r="D21">
         <v>0</v>
       </c>
@@ -21623,6 +21678,9 @@
       <c r="B23" t="s">
         <v>24</v>
       </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
       <c r="D23">
         <v>0</v>
       </c>
@@ -21658,6 +21716,9 @@
       <c r="B24" t="s">
         <v>25</v>
       </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
       <c r="D24">
         <v>0</v>
       </c>
@@ -21693,6 +21754,9 @@
       <c r="B25" t="s">
         <v>26</v>
       </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
       <c r="D25">
         <v>0</v>
       </c>
@@ -21728,6 +21792,9 @@
       <c r="B26" t="s">
         <v>27</v>
       </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
       <c r="D26">
         <v>0</v>
       </c>
@@ -21763,6 +21830,9 @@
       <c r="B27" t="s">
         <v>28</v>
       </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
       <c r="D27">
         <v>0</v>
       </c>
@@ -21798,6 +21868,9 @@
       <c r="B28" t="s">
         <v>29</v>
       </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
       <c r="D28">
         <v>0</v>
       </c>
@@ -21833,6 +21906,9 @@
       <c r="B29" t="s">
         <v>30</v>
       </c>
+      <c r="C29" t="s">
+        <v>71</v>
+      </c>
       <c r="D29">
         <v>0</v>
       </c>
@@ -21868,6 +21944,9 @@
       <c r="B30" t="s">
         <v>31</v>
       </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
       <c r="D30">
         <v>0</v>
       </c>
@@ -21903,6 +21982,9 @@
       <c r="B31" t="s">
         <v>32</v>
       </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
       <c r="D31">
         <v>0</v>
       </c>
@@ -21938,6 +22020,9 @@
       <c r="B32" t="s">
         <v>33</v>
       </c>
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
       <c r="D32">
         <v>0</v>
       </c>
@@ -21973,6 +22058,9 @@
       <c r="B33" t="s">
         <v>34</v>
       </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
       <c r="D33">
         <v>0</v>
       </c>
@@ -22008,6 +22096,9 @@
       <c r="B34" t="s">
         <v>35</v>
       </c>
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
       <c r="D34">
         <v>0</v>
       </c>
@@ -22043,6 +22134,9 @@
       <c r="B35" t="s">
         <v>36</v>
       </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
       <c r="D35">
         <v>0</v>
       </c>
@@ -22078,6 +22172,9 @@
       <c r="B36" t="s">
         <v>37</v>
       </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
       <c r="D36">
         <v>0</v>
       </c>
@@ -22113,6 +22210,9 @@
       <c r="B37" t="s">
         <v>38</v>
       </c>
+      <c r="C37" t="s">
+        <v>71</v>
+      </c>
       <c r="D37">
         <v>0</v>
       </c>
@@ -22148,6 +22248,9 @@
       <c r="B38" t="s">
         <v>39</v>
       </c>
+      <c r="C38" t="s">
+        <v>71</v>
+      </c>
       <c r="D38">
         <v>0</v>
       </c>
@@ -22183,6 +22286,9 @@
       <c r="B39" t="s">
         <v>40</v>
       </c>
+      <c r="C39" t="s">
+        <v>71</v>
+      </c>
       <c r="D39">
         <v>0</v>
       </c>
@@ -22218,6 +22324,9 @@
       <c r="B40" t="s">
         <v>41</v>
       </c>
+      <c r="C40" t="s">
+        <v>71</v>
+      </c>
       <c r="D40">
         <v>0</v>
       </c>
@@ -22253,6 +22362,9 @@
       <c r="B41" t="s">
         <v>63</v>
       </c>
+      <c r="C41" t="s">
+        <v>71</v>
+      </c>
       <c r="D41" t="s">
         <v>80</v>
       </c>
@@ -22288,6 +22400,9 @@
       <c r="B42" t="s">
         <v>42</v>
       </c>
+      <c r="C42" t="s">
+        <v>71</v>
+      </c>
       <c r="D42">
         <v>0</v>
       </c>
@@ -22323,6 +22438,9 @@
       <c r="B43" t="s">
         <v>43</v>
       </c>
+      <c r="C43" t="s">
+        <v>71</v>
+      </c>
       <c r="D43">
         <v>0</v>
       </c>
@@ -22358,6 +22476,9 @@
       <c r="B44" t="s">
         <v>44</v>
       </c>
+      <c r="C44" t="s">
+        <v>71</v>
+      </c>
       <c r="D44">
         <v>0</v>
       </c>
@@ -22393,6 +22514,9 @@
       <c r="B45" t="s">
         <v>64</v>
       </c>
+      <c r="C45" t="s">
+        <v>71</v>
+      </c>
       <c r="D45" t="s">
         <v>80</v>
       </c>
@@ -22466,6 +22590,9 @@
       <c r="B47" t="s">
         <v>46</v>
       </c>
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
       <c r="D47">
         <v>0</v>
       </c>
@@ -22501,6 +22628,9 @@
       <c r="B48" t="s">
         <v>47</v>
       </c>
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
       <c r="D48">
         <v>0</v>
       </c>
@@ -22536,6 +22666,9 @@
       <c r="B49" t="s">
         <v>48</v>
       </c>
+      <c r="C49" t="s">
+        <v>71</v>
+      </c>
       <c r="D49">
         <v>0</v>
       </c>
@@ -22571,6 +22704,9 @@
       <c r="B50" t="s">
         <v>49</v>
       </c>
+      <c r="C50" t="s">
+        <v>71</v>
+      </c>
       <c r="D50">
         <v>0</v>
       </c>
@@ -22606,6 +22742,9 @@
       <c r="B51" t="s">
         <v>50</v>
       </c>
+      <c r="C51" t="s">
+        <v>71</v>
+      </c>
       <c r="D51">
         <v>0</v>
       </c>
@@ -22641,6 +22780,9 @@
       <c r="B52" t="s">
         <v>51</v>
       </c>
+      <c r="C52" t="s">
+        <v>71</v>
+      </c>
       <c r="D52">
         <v>0</v>
       </c>
@@ -22676,6 +22818,9 @@
       <c r="B53" t="s">
         <v>52</v>
       </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
       <c r="D53">
         <v>0</v>
       </c>
@@ -22711,6 +22856,9 @@
       <c r="B54" t="s">
         <v>53</v>
       </c>
+      <c r="C54" t="s">
+        <v>71</v>
+      </c>
       <c r="D54">
         <v>0</v>
       </c>
@@ -22746,6 +22894,9 @@
       <c r="B55" t="s">
         <v>54</v>
       </c>
+      <c r="C55" t="s">
+        <v>71</v>
+      </c>
       <c r="D55">
         <v>0</v>
       </c>
@@ -22781,6 +22932,9 @@
       <c r="B56" t="s">
         <v>55</v>
       </c>
+      <c r="C56" t="s">
+        <v>71</v>
+      </c>
       <c r="D56">
         <v>0</v>
       </c>
@@ -22816,6 +22970,9 @@
       <c r="B57" t="s">
         <v>56</v>
       </c>
+      <c r="C57" t="s">
+        <v>71</v>
+      </c>
       <c r="D57">
         <v>0</v>
       </c>
@@ -22851,6 +23008,9 @@
       <c r="B58" t="s">
         <v>57</v>
       </c>
+      <c r="C58" t="s">
+        <v>71</v>
+      </c>
       <c r="D58">
         <v>0</v>
       </c>
@@ -22886,6 +23046,9 @@
       <c r="B59" t="s">
         <v>58</v>
       </c>
+      <c r="C59" t="s">
+        <v>71</v>
+      </c>
       <c r="D59">
         <v>0</v>
       </c>
@@ -22921,6 +23084,9 @@
       <c r="B60" t="s">
         <v>59</v>
       </c>
+      <c r="C60" t="s">
+        <v>71</v>
+      </c>
       <c r="D60">
         <v>0</v>
       </c>
@@ -22956,6 +23122,9 @@
       <c r="B61" t="s">
         <v>60</v>
       </c>
+      <c r="C61" t="s">
+        <v>71</v>
+      </c>
       <c r="D61">
         <v>0</v>
       </c>
@@ -22991,6 +23160,9 @@
       <c r="B62" t="s">
         <v>4</v>
       </c>
+      <c r="C62" t="s">
+        <v>71</v>
+      </c>
       <c r="D62">
         <v>0</v>
       </c>
@@ -23026,6 +23198,9 @@
       <c r="B63" t="s">
         <v>5</v>
       </c>
+      <c r="C63" t="s">
+        <v>71</v>
+      </c>
       <c r="D63">
         <v>0</v>
       </c>
@@ -23061,6 +23236,9 @@
       <c r="B64" t="s">
         <v>6</v>
       </c>
+      <c r="C64" t="s">
+        <v>71</v>
+      </c>
       <c r="D64">
         <v>0</v>
       </c>
@@ -23172,6 +23350,9 @@
       <c r="B67" t="s">
         <v>9</v>
       </c>
+      <c r="C67" t="s">
+        <v>71</v>
+      </c>
       <c r="D67">
         <v>0</v>
       </c>
@@ -23207,6 +23388,9 @@
       <c r="B68" t="s">
         <v>10</v>
       </c>
+      <c r="C68" t="s">
+        <v>71</v>
+      </c>
       <c r="D68">
         <v>0</v>
       </c>
@@ -23242,6 +23426,9 @@
       <c r="B69" t="s">
         <v>11</v>
       </c>
+      <c r="C69" t="s">
+        <v>71</v>
+      </c>
       <c r="D69">
         <v>0</v>
       </c>
@@ -23277,6 +23464,9 @@
       <c r="B70" t="s">
         <v>12</v>
       </c>
+      <c r="C70" t="s">
+        <v>71</v>
+      </c>
       <c r="D70">
         <v>0</v>
       </c>
@@ -23312,6 +23502,9 @@
       <c r="B71" t="s">
         <v>13</v>
       </c>
+      <c r="C71" t="s">
+        <v>71</v>
+      </c>
       <c r="D71">
         <v>0</v>
       </c>
@@ -23385,6 +23578,9 @@
       <c r="B73" t="s">
         <v>15</v>
       </c>
+      <c r="C73" t="s">
+        <v>71</v>
+      </c>
       <c r="D73">
         <v>0</v>
       </c>
@@ -23420,6 +23616,9 @@
       <c r="B74" t="s">
         <v>16</v>
       </c>
+      <c r="C74" t="s">
+        <v>71</v>
+      </c>
       <c r="D74">
         <v>0</v>
       </c>
@@ -23455,6 +23654,9 @@
       <c r="B75" t="s">
         <v>17</v>
       </c>
+      <c r="C75" t="s">
+        <v>71</v>
+      </c>
       <c r="D75">
         <v>0</v>
       </c>
@@ -23528,6 +23730,9 @@
       <c r="B77" t="s">
         <v>19</v>
       </c>
+      <c r="C77" t="s">
+        <v>71</v>
+      </c>
       <c r="D77">
         <v>0</v>
       </c>
@@ -23563,6 +23768,9 @@
       <c r="B78" t="s">
         <v>20</v>
       </c>
+      <c r="C78" t="s">
+        <v>71</v>
+      </c>
       <c r="D78">
         <v>0</v>
       </c>
@@ -23598,6 +23806,9 @@
       <c r="B79" t="s">
         <v>62</v>
       </c>
+      <c r="C79" t="s">
+        <v>71</v>
+      </c>
       <c r="D79">
         <v>0</v>
       </c>
@@ -23633,6 +23844,9 @@
       <c r="B80" t="s">
         <v>21</v>
       </c>
+      <c r="C80" t="s">
+        <v>71</v>
+      </c>
       <c r="D80">
         <v>0</v>
       </c>
@@ -23668,6 +23882,9 @@
       <c r="B81" t="s">
         <v>22</v>
       </c>
+      <c r="C81" t="s">
+        <v>71</v>
+      </c>
       <c r="D81">
         <v>0</v>
       </c>
@@ -23741,6 +23958,9 @@
       <c r="B83" t="s">
         <v>24</v>
       </c>
+      <c r="C83" t="s">
+        <v>71</v>
+      </c>
       <c r="D83">
         <v>0</v>
       </c>
@@ -23776,6 +23996,9 @@
       <c r="B84" t="s">
         <v>25</v>
       </c>
+      <c r="C84" t="s">
+        <v>71</v>
+      </c>
       <c r="D84">
         <v>0</v>
       </c>
@@ -23811,6 +24034,9 @@
       <c r="B85" t="s">
         <v>26</v>
       </c>
+      <c r="C85" t="s">
+        <v>71</v>
+      </c>
       <c r="D85">
         <v>0</v>
       </c>
@@ -23846,6 +24072,9 @@
       <c r="B86" t="s">
         <v>27</v>
       </c>
+      <c r="C86" t="s">
+        <v>71</v>
+      </c>
       <c r="D86">
         <v>0</v>
       </c>
@@ -23881,6 +24110,9 @@
       <c r="B87" t="s">
         <v>28</v>
       </c>
+      <c r="C87" t="s">
+        <v>71</v>
+      </c>
       <c r="D87">
         <v>0</v>
       </c>
@@ -23916,6 +24148,9 @@
       <c r="B88" t="s">
         <v>29</v>
       </c>
+      <c r="C88" t="s">
+        <v>71</v>
+      </c>
       <c r="D88">
         <v>0</v>
       </c>
@@ -23951,6 +24186,9 @@
       <c r="B89" t="s">
         <v>30</v>
       </c>
+      <c r="C89" t="s">
+        <v>71</v>
+      </c>
       <c r="D89">
         <v>0</v>
       </c>
@@ -23986,6 +24224,9 @@
       <c r="B90" t="s">
         <v>31</v>
       </c>
+      <c r="C90" t="s">
+        <v>71</v>
+      </c>
       <c r="D90">
         <v>0</v>
       </c>
@@ -24021,6 +24262,9 @@
       <c r="B91" t="s">
         <v>32</v>
       </c>
+      <c r="C91" t="s">
+        <v>71</v>
+      </c>
       <c r="D91">
         <v>0</v>
       </c>
@@ -24056,6 +24300,9 @@
       <c r="B92" t="s">
         <v>33</v>
       </c>
+      <c r="C92" t="s">
+        <v>71</v>
+      </c>
       <c r="D92">
         <v>0</v>
       </c>
@@ -24091,6 +24338,9 @@
       <c r="B93" t="s">
         <v>34</v>
       </c>
+      <c r="C93" t="s">
+        <v>71</v>
+      </c>
       <c r="D93">
         <v>0</v>
       </c>
@@ -24126,6 +24376,9 @@
       <c r="B94" t="s">
         <v>35</v>
       </c>
+      <c r="C94" t="s">
+        <v>71</v>
+      </c>
       <c r="D94">
         <v>0</v>
       </c>
@@ -24161,6 +24414,9 @@
       <c r="B95" t="s">
         <v>36</v>
       </c>
+      <c r="C95" t="s">
+        <v>71</v>
+      </c>
       <c r="D95">
         <v>0</v>
       </c>
@@ -24196,6 +24452,9 @@
       <c r="B96" t="s">
         <v>37</v>
       </c>
+      <c r="C96" t="s">
+        <v>71</v>
+      </c>
       <c r="D96">
         <v>0</v>
       </c>
@@ -24231,6 +24490,9 @@
       <c r="B97" t="s">
         <v>38</v>
       </c>
+      <c r="C97" t="s">
+        <v>71</v>
+      </c>
       <c r="D97">
         <v>0</v>
       </c>
@@ -24266,6 +24528,9 @@
       <c r="B98" t="s">
         <v>39</v>
       </c>
+      <c r="C98" t="s">
+        <v>71</v>
+      </c>
       <c r="D98">
         <v>0</v>
       </c>
@@ -24301,6 +24566,9 @@
       <c r="B99" t="s">
         <v>40</v>
       </c>
+      <c r="C99" t="s">
+        <v>71</v>
+      </c>
       <c r="D99">
         <v>0</v>
       </c>
@@ -24336,6 +24604,9 @@
       <c r="B100" t="s">
         <v>41</v>
       </c>
+      <c r="C100" t="s">
+        <v>71</v>
+      </c>
       <c r="D100">
         <v>0</v>
       </c>
@@ -24371,6 +24642,9 @@
       <c r="B101" t="s">
         <v>63</v>
       </c>
+      <c r="C101" t="s">
+        <v>71</v>
+      </c>
       <c r="D101">
         <v>0</v>
       </c>
@@ -24406,6 +24680,9 @@
       <c r="B102" t="s">
         <v>42</v>
       </c>
+      <c r="C102" t="s">
+        <v>71</v>
+      </c>
       <c r="D102">
         <v>0</v>
       </c>
@@ -24441,6 +24718,9 @@
       <c r="B103" t="s">
         <v>43</v>
       </c>
+      <c r="C103" t="s">
+        <v>71</v>
+      </c>
       <c r="D103">
         <v>0</v>
       </c>
@@ -24476,6 +24756,9 @@
       <c r="B104" t="s">
         <v>44</v>
       </c>
+      <c r="C104" t="s">
+        <v>71</v>
+      </c>
       <c r="D104">
         <v>0</v>
       </c>
@@ -24549,6 +24832,9 @@
       <c r="B106" t="s">
         <v>45</v>
       </c>
+      <c r="C106" t="s">
+        <v>71</v>
+      </c>
       <c r="D106">
         <v>0</v>
       </c>
@@ -24584,6 +24870,9 @@
       <c r="B107" t="s">
         <v>46</v>
       </c>
+      <c r="C107" t="s">
+        <v>71</v>
+      </c>
       <c r="D107">
         <v>0</v>
       </c>
@@ -24619,6 +24908,9 @@
       <c r="B108" t="s">
         <v>47</v>
       </c>
+      <c r="C108" t="s">
+        <v>71</v>
+      </c>
       <c r="D108">
         <v>0</v>
       </c>
@@ -24654,6 +24946,9 @@
       <c r="B109" t="s">
         <v>48</v>
       </c>
+      <c r="C109" t="s">
+        <v>71</v>
+      </c>
       <c r="D109">
         <v>0</v>
       </c>
@@ -24689,6 +24984,9 @@
       <c r="B110" t="s">
         <v>49</v>
       </c>
+      <c r="C110" t="s">
+        <v>71</v>
+      </c>
       <c r="D110">
         <v>0</v>
       </c>
@@ -24724,6 +25022,9 @@
       <c r="B111" t="s">
         <v>50</v>
       </c>
+      <c r="C111" t="s">
+        <v>71</v>
+      </c>
       <c r="D111">
         <v>0</v>
       </c>
@@ -24759,6 +25060,9 @@
       <c r="B112" t="s">
         <v>51</v>
       </c>
+      <c r="C112" t="s">
+        <v>71</v>
+      </c>
       <c r="D112">
         <v>0</v>
       </c>
@@ -24794,6 +25098,9 @@
       <c r="B113" t="s">
         <v>52</v>
       </c>
+      <c r="C113" t="s">
+        <v>71</v>
+      </c>
       <c r="D113">
         <v>0</v>
       </c>
@@ -24829,6 +25136,9 @@
       <c r="B114" t="s">
         <v>53</v>
       </c>
+      <c r="C114" t="s">
+        <v>71</v>
+      </c>
       <c r="D114">
         <v>0</v>
       </c>
@@ -24864,6 +25174,9 @@
       <c r="B115" t="s">
         <v>54</v>
       </c>
+      <c r="C115" t="s">
+        <v>71</v>
+      </c>
       <c r="D115">
         <v>0</v>
       </c>
@@ -24899,6 +25212,9 @@
       <c r="B116" t="s">
         <v>55</v>
       </c>
+      <c r="C116" t="s">
+        <v>71</v>
+      </c>
       <c r="D116">
         <v>0</v>
       </c>
@@ -24934,6 +25250,9 @@
       <c r="B117" t="s">
         <v>56</v>
       </c>
+      <c r="C117" t="s">
+        <v>71</v>
+      </c>
       <c r="D117">
         <v>0</v>
       </c>
@@ -24969,6 +25288,9 @@
       <c r="B118" t="s">
         <v>57</v>
       </c>
+      <c r="C118" t="s">
+        <v>71</v>
+      </c>
       <c r="D118">
         <v>0</v>
       </c>
@@ -25004,6 +25326,9 @@
       <c r="B119" t="s">
         <v>58</v>
       </c>
+      <c r="C119" t="s">
+        <v>71</v>
+      </c>
       <c r="D119">
         <v>0</v>
       </c>
@@ -25039,6 +25364,9 @@
       <c r="B120" t="s">
         <v>59</v>
       </c>
+      <c r="C120" t="s">
+        <v>71</v>
+      </c>
       <c r="D120">
         <v>0</v>
       </c>
@@ -25074,6 +25402,9 @@
       <c r="B121" t="s">
         <v>60</v>
       </c>
+      <c r="C121" t="s">
+        <v>71</v>
+      </c>
       <c r="D121">
         <v>0</v>
       </c>
@@ -25103,7 +25434,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J128">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J128">
     <sortCondition ref="A2:A128"/>
     <sortCondition ref="B2:B128"/>
   </sortState>

</xml_diff>